<commit_message>
excel updated, a carrier phase shift is added and simulation results are taken.
</commit_message>
<xml_diff>
--- a/Simulations/MATLAB-SIMULINK/3-Phase-Modelling/New_models/Simulation_results_VAB.xlsx
+++ b/Simulations/MATLAB-SIMULINK/3-Phase-Modelling/New_models/Simulation_results_VAB.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20376"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E8562C-85EB-4E38-8A92-986DE9FBE45C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9B20C4-2764-4DF1-8848-228341890CA9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
   <si>
     <t>Vdc=100V</t>
   </si>
@@ -63,6 +64,36 @@
   </si>
   <si>
     <t>fsw-2fo-anal</t>
+  </si>
+  <si>
+    <t>carrier 40 degree</t>
+  </si>
+  <si>
+    <t>Vout</t>
+  </si>
+  <si>
+    <t>250V DC</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>diff</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>deviation %</t>
+  </si>
+  <si>
+    <t>analitik method</t>
+  </si>
+  <si>
+    <t>ratio</t>
   </si>
 </sst>
 </file>
@@ -2760,6 +2791,723 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.14508652787060422"/>
+          <c:y val="2.3631219836911296E-2"/>
+          <c:w val="0.65399067728757365"/>
+          <c:h val="0.65292691342593434"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>fo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$B$5:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.23</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30.47</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45.73</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60.95</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>75.959999999999994</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>91.07</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>106.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>121.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>136.80000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>152.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-AEB9-442C-9CF8-19F938A565F0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>fsw-2fm</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$C$5:$C$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4385</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7210000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.87</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.53</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14.64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19.260000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>30.15</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>35.94</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-AEB9-442C-9CF8-19F938A565F0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>fsw</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$D$5:$D$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>75.11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>74.58</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>73.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70.930000000000007</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>67.84</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64.209999999999994</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>59.84</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>54.88</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>49.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42.79</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>54.45</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-AEB9-442C-9CF8-19F938A565F0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>fsw+2fm</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$E$5:$E$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.67700000000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.694</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.9859999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.48</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.86</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>29.63</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>37.590000000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>36.14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-AEB9-442C-9CF8-19F938A565F0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$F$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vout</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$F$5:$F$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>46.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45.86</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45.03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43.79</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42.35</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41.09</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>39.869999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>39.229999999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40.090000000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41.68</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43.97</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-AEB9-442C-9CF8-19F938A565F0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="740359120"/>
+        <c:axId val="672383168"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="740359120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="672383168"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="672383168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="740359120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.8460499207103449"/>
+          <c:y val="0.22263910971784479"/>
+          <c:w val="0.12620578622708065"/>
+          <c:h val="0.34031967316201273"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2920,6 +3668,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -4430,6 +5218,509 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5092,6 +6383,49 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>548640</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>49364</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>169296</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{630061E7-C780-424A-9BAD-2B05EC306332}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5618,8 +6952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C694F671-CB78-4743-A587-43F6FE16E557}">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6044,4 +7378,411 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9531250-C6B7-4D06-B971-B1C9F17D5481}">
+  <dimension ref="A1:H22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>75.11</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>46.2</v>
+      </c>
+      <c r="G5">
+        <f>SQRT(C5*C5+D5*D5+E5*E5)</f>
+        <v>75.11</v>
+      </c>
+      <c r="H5">
+        <f>G5/F5</f>
+        <v>1.6257575757575757</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="B6" s="1">
+        <v>15.23</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.4385</v>
+      </c>
+      <c r="D6" s="1">
+        <v>74.58</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.67700000000000005</v>
+      </c>
+      <c r="F6" s="1">
+        <v>45.86</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ref="G6:G15" si="0">SQRT(C6*C6+D6*D6+E6*E6)</f>
+        <v>74.584361707062953</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ref="H6:H15" si="1">G6/F6</f>
+        <v>1.6263489251431085</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>30.47</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1.7210000000000001</v>
+      </c>
+      <c r="D7" s="1">
+        <v>73.2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2.694</v>
+      </c>
+      <c r="F7" s="1">
+        <v>45.03</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>73.269771918575003</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>1.6271323988135689</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="B8" s="1">
+        <v>45.73</v>
+      </c>
+      <c r="C8" s="1">
+        <v>3.87</v>
+      </c>
+      <c r="D8" s="1">
+        <v>70.930000000000007</v>
+      </c>
+      <c r="E8" s="1">
+        <v>5.9859999999999998</v>
+      </c>
+      <c r="F8" s="1">
+        <v>43.79</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>71.287263911585228</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>1.6279347776109896</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="B9" s="1">
+        <v>60.95</v>
+      </c>
+      <c r="C9" s="1">
+        <v>6.8</v>
+      </c>
+      <c r="D9" s="1">
+        <v>67.84</v>
+      </c>
+      <c r="E9" s="1">
+        <v>10.48</v>
+      </c>
+      <c r="F9" s="1">
+        <v>42.35</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>68.980692950998986</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>1.6288239185595983</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="B10" s="1">
+        <v>75.959999999999994</v>
+      </c>
+      <c r="C10" s="1">
+        <v>10.53</v>
+      </c>
+      <c r="D10" s="1">
+        <v>64.209999999999994</v>
+      </c>
+      <c r="E10" s="1">
+        <v>15.86</v>
+      </c>
+      <c r="F10" s="1">
+        <v>41.09</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>66.972715339905392</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>1.6299030260380964</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="B11" s="1">
+        <v>91.07</v>
+      </c>
+      <c r="C11" s="1">
+        <v>14.64</v>
+      </c>
+      <c r="D11" s="1">
+        <v>59.84</v>
+      </c>
+      <c r="E11" s="1">
+        <v>22.3</v>
+      </c>
+      <c r="F11" s="1">
+        <v>39.869999999999997</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>65.516755108903254</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>1.6432594710033424</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="B12" s="1">
+        <v>106.3</v>
+      </c>
+      <c r="C12" s="1">
+        <v>19.260000000000002</v>
+      </c>
+      <c r="D12" s="1">
+        <v>54.88</v>
+      </c>
+      <c r="E12" s="1">
+        <v>29.63</v>
+      </c>
+      <c r="F12" s="1">
+        <v>39.229999999999997</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>65.274029291901385</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>1.6638804305863215</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="B13" s="1">
+        <v>121.6</v>
+      </c>
+      <c r="C13" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="D13" s="1">
+        <v>49.1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>37.590000000000003</v>
+      </c>
+      <c r="F13" s="1">
+        <v>40.090000000000003</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>66.51366852008691</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>1.6591087183858044</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B14" s="1">
+        <v>136.80000000000001</v>
+      </c>
+      <c r="C14" s="1">
+        <v>30.15</v>
+      </c>
+      <c r="D14" s="1">
+        <v>42.79</v>
+      </c>
+      <c r="E14" s="1">
+        <v>45.9</v>
+      </c>
+      <c r="F14" s="1">
+        <v>41.68</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>69.619082154248488</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>1.6703234681921422</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1">
+        <v>152.1</v>
+      </c>
+      <c r="C15" s="1">
+        <v>35.94</v>
+      </c>
+      <c r="D15" s="1">
+        <v>54.45</v>
+      </c>
+      <c r="E15" s="1">
+        <v>36.14</v>
+      </c>
+      <c r="F15" s="1">
+        <v>43.97</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>74.58274398277392</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>1.6962188761149402</v>
+      </c>
+    </row>
+    <row r="18" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18">
+        <f>MAX(F5:F15)</f>
+        <v>46.2</v>
+      </c>
+    </row>
+    <row r="19" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19">
+        <f>MIN(F5:F15)</f>
+        <v>39.229999999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20">
+        <f>F18-F19</f>
+        <v>6.970000000000006</v>
+      </c>
+    </row>
+    <row r="21" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E21" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21">
+        <f>AVERAGE(F5:F15)</f>
+        <v>42.650909090909089</v>
+      </c>
+    </row>
+    <row r="22" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E22" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22">
+        <f>100*F20/F21</f>
+        <v>16.341972887714228</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
For a single carrier phase shift value (40 degree), we obtain the almost constant output voltage along the all modulation index. We also validate the results experimentally.
</commit_message>
<xml_diff>
--- a/Simulations/MATLAB-SIMULINK/3-Phase-Modelling/New_models/Simulation_results_VAB.xlsx
+++ b/Simulations/MATLAB-SIMULINK/3-Phase-Modelling/New_models/Simulation_results_VAB.xlsx
@@ -3,14 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20376"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9B20C4-2764-4DF1-8848-228341890CA9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F513CC0D-5FCA-485D-80D9-D06AE58C0760}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
   <si>
     <t>Vdc=100V</t>
   </si>
@@ -95,12 +97,33 @@
   <si>
     <t>ratio</t>
   </si>
+  <si>
+    <t>Vin</t>
+  </si>
+  <si>
+    <t>Iin</t>
+  </si>
+  <si>
+    <t>Vcap</t>
+  </si>
+  <si>
+    <t>Itx</t>
+  </si>
+  <si>
+    <t>Test sonuçları 40 derece carrier</t>
+  </si>
+  <si>
+    <t>80 kHz</t>
+  </si>
+  <si>
+    <t>analitik Vout</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,13 +146,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -141,10 +176,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -156,8 +192,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3508,6 +3549,504 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16964208805035"/>
+          <c:y val="3.9764867520369319E-2"/>
+          <c:w val="0.65399067728757365"/>
+          <c:h val="0.65292691342593434"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet5!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vout</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet5!$A$4:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet5!$E$4:$E$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>11.57</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.52</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.34</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.78</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.27</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.23</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.44</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.68</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-62CF-4A59-B631-5663EF1ED236}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet5!$G$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>analitik Vout</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet5!$H$22:$H$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>12.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-62CF-4A59-B631-5663EF1ED236}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="740359120"/>
+        <c:axId val="672383168"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="740359120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="672383168"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="672383168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="740359120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.8460499207103449"/>
+          <c:y val="0.22263910971784479"/>
+          <c:w val="0.15395007928965507"/>
+          <c:h val="0.13612786926480511"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3708,6 +4247,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -5721,6 +6300,509 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6426,6 +7508,49 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>510540</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>79844</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>161676</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{097C6E01-337F-441E-8C9F-3C195F31DF9E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -6692,7 +7817,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A5" sqref="A5:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6952,8 +8077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C694F671-CB78-4743-A587-43F6FE16E557}">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:E16"/>
+    <sheetView topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="X41" sqref="X41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7382,10 +8507,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9531250-C6B7-4D06-B971-B1C9F17D5481}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7736,7 +8861,7 @@
         <v>1.6962188761149402</v>
       </c>
     </row>
-    <row r="18" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E18" t="s">
         <v>17</v>
       </c>
@@ -7745,7 +8870,7 @@
         <v>46.2</v>
       </c>
     </row>
-    <row r="19" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E19" t="s">
         <v>18</v>
       </c>
@@ -7754,7 +8879,8 @@
         <v>39.229999999999997</v>
       </c>
     </row>
-    <row r="20" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
       <c r="E20" t="s">
         <v>19</v>
       </c>
@@ -7763,7 +8889,8 @@
         <v>6.970000000000006</v>
       </c>
     </row>
-    <row r="21" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
       <c r="E21" t="s">
         <v>20</v>
       </c>
@@ -7772,13 +8899,1241 @@
         <v>42.650909090909089</v>
       </c>
     </row>
-    <row r="22" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
       <c r="E22" t="s">
         <v>21</v>
       </c>
       <c r="F22">
         <f>100*F20/F21</f>
         <v>16.341972887714228</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{554443A8-792B-40E6-9CA4-BD6F9E1517FD}">
+  <dimension ref="A3:N24"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <f>ROUND(K4,1)</f>
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <f>ROUND(L4,1)</f>
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <f>ROUND(M4,1)</f>
+        <v>30.8</v>
+      </c>
+      <c r="E4">
+        <f>ROUND(N4,1)</f>
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1">
+        <v>30.792631549049201</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="B5">
+        <f t="shared" ref="B5:B24" si="0">ROUND(K5,1)</f>
+        <v>4.3</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:C24" si="1">ROUND(L5,1)</f>
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D5:D24" si="2">ROUND(M5,1)</f>
+        <v>30.7</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E5:E24" si="3">ROUND(N5,1)</f>
+        <v>0.1</v>
+      </c>
+      <c r="K5" s="1">
+        <v>4.3301270189221901</v>
+      </c>
+      <c r="L5" s="1">
+        <v>4.4599412040141798E-2</v>
+      </c>
+      <c r="M5" s="1">
+        <v>30.745163745196599</v>
+      </c>
+      <c r="N5" s="1">
+        <v>6.8330263519448597E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="2"/>
+        <v>30.6</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="3"/>
+        <v>0.3</v>
+      </c>
+      <c r="K6" s="1">
+        <v>8.6602540378443909</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0.178122660282621</v>
+      </c>
+      <c r="M6" s="1">
+        <v>30.602979834140999</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0.27289974820614299</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>0.4</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="2"/>
+        <v>30.4</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="3"/>
+        <v>0.6</v>
+      </c>
+      <c r="K7" s="1">
+        <v>12.9903810567666</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0.39974637058462198</v>
+      </c>
+      <c r="M7" s="1">
+        <v>30.366737189620402</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0.61244697168665896</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="B8" s="6">
+        <f t="shared" si="0"/>
+        <v>17.3</v>
+      </c>
+      <c r="C8" s="6">
+        <f t="shared" si="1"/>
+        <v>0.7</v>
+      </c>
+      <c r="D8" s="6">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="E8" s="6">
+        <f t="shared" si="3"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K8" s="1">
+        <v>17.320508075688799</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0.70810354186486901</v>
+      </c>
+      <c r="M8" s="1">
+        <v>30.0375276813858</v>
+      </c>
+      <c r="N8" s="1">
+        <v>1.0848775667969</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>21.7</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="2"/>
+        <v>29.6</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="3"/>
+        <v>1.7</v>
+      </c>
+      <c r="K9" s="1">
+        <v>21.650635094611001</v>
+      </c>
+      <c r="L9" s="1">
+        <v>1.10129144787831</v>
+      </c>
+      <c r="M9" s="1">
+        <v>29.6168720667436</v>
+      </c>
+      <c r="N9" s="1">
+        <v>1.6872763878032599</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>1.6</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="2"/>
+        <v>29.1</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="3"/>
+        <v>2.4</v>
+      </c>
+      <c r="K10" s="1">
+        <v>25.980762113533199</v>
+      </c>
+      <c r="L10" s="1">
+        <v>1.57688263596981</v>
+      </c>
+      <c r="M10" s="1">
+        <v>29.106712181114101</v>
+      </c>
+      <c r="N10" s="1">
+        <v>2.4159243614709598</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>30.3</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>2.1</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="2"/>
+        <v>28.5</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="3"/>
+        <v>3.3</v>
+      </c>
+      <c r="K11" s="1">
+        <v>30.310889132455401</v>
+      </c>
+      <c r="L11" s="1">
+        <v>2.1319389595182598</v>
+      </c>
+      <c r="M11" s="1">
+        <v>28.5094009697223</v>
+      </c>
+      <c r="N11" s="1">
+        <v>3.26631998601564</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>34.6</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>2.8</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="2"/>
+        <v>27.8</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="3"/>
+        <v>4.2</v>
+      </c>
+      <c r="K12" s="1">
+        <v>34.641016151377499</v>
+      </c>
+      <c r="L12" s="1">
+        <v>2.76302856332893</v>
+      </c>
+      <c r="M12" s="1">
+        <v>27.827690414170998</v>
+      </c>
+      <c r="N12" s="1">
+        <v>4.23320535423428</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>3.5</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="2"/>
+        <v>27.1</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="3"/>
+        <v>5.3</v>
+      </c>
+      <c r="K13" s="1">
+        <v>38.971143170299698</v>
+      </c>
+      <c r="L13" s="1">
+        <v>3.46624572424495</v>
+      </c>
+      <c r="M13" s="1">
+        <v>27.064717418976699</v>
+      </c>
+      <c r="N13" s="1">
+        <v>5.3105965510855198</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="B14" s="6">
+        <f t="shared" si="0"/>
+        <v>43.3</v>
+      </c>
+      <c r="C14" s="6">
+        <f t="shared" si="1"/>
+        <v>4.2</v>
+      </c>
+      <c r="D14" s="6">
+        <f t="shared" si="2"/>
+        <v>26.2</v>
+      </c>
+      <c r="E14" s="6">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="K14" s="1">
+        <v>43.301270189221903</v>
+      </c>
+      <c r="L14" s="1">
+        <v>4.2372334328268799</v>
+      </c>
+      <c r="M14" s="1">
+        <v>26.223987734123799</v>
+      </c>
+      <c r="N14" s="1">
+        <v>6.4918182508299704</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>47.6</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="2"/>
+        <v>25.3</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="3"/>
+        <v>7.8</v>
+      </c>
+      <c r="K15">
+        <v>47.631397208144101</v>
+      </c>
+      <c r="L15">
+        <v>5.0712085861865397</v>
+      </c>
+      <c r="M15">
+        <v>25.309358000242401</v>
+      </c>
+      <c r="N15">
+        <v>7.7695423146909004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="2"/>
+        <v>24.3</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="3"/>
+        <v>9.1</v>
+      </c>
+      <c r="K16">
+        <v>51.961524227066299</v>
+      </c>
+      <c r="L16">
+        <v>5.9629896470497599</v>
+      </c>
+      <c r="M16">
+        <v>24.3250160130866</v>
+      </c>
+      <c r="N16">
+        <v>9.1358301669969393</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>56.3</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>6.9</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="2"/>
+        <v>23.3</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="3"/>
+        <v>10.6</v>
+      </c>
+      <c r="K17">
+        <v>56.291651245988497</v>
+      </c>
+      <c r="L17">
+        <v>6.9070266099481703</v>
+      </c>
+      <c r="M17">
+        <v>23.275459313523299</v>
+      </c>
+      <c r="N17">
+        <v>10.582178706051399</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="B18" s="6">
+        <f t="shared" si="0"/>
+        <v>60.6</v>
+      </c>
+      <c r="C18" s="6">
+        <f t="shared" si="1"/>
+        <v>7.9</v>
+      </c>
+      <c r="D18" s="6">
+        <f t="shared" si="2"/>
+        <v>22.2</v>
+      </c>
+      <c r="E18" s="6">
+        <f t="shared" si="3"/>
+        <v>12.1</v>
+      </c>
+      <c r="K18">
+        <v>60.621778264910702</v>
+      </c>
+      <c r="L18">
+        <v>7.8974331021847703</v>
+      </c>
+      <c r="M18">
+        <v>22.165472218191301</v>
+      </c>
+      <c r="N18">
+        <v>12.099569485665</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>8.9</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="3"/>
+        <v>13.7</v>
+      </c>
+      <c r="K19">
+        <v>64.9519052838329</v>
+      </c>
+      <c r="L19">
+        <v>8.92802043495848</v>
+      </c>
+      <c r="M19">
+        <v>21.000101414296399</v>
+      </c>
+      <c r="N19">
+        <v>13.6785208845052</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>69.3</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="2"/>
+        <v>19.8</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="3"/>
+        <v>15.3</v>
+      </c>
+      <c r="K20">
+        <v>69.282032302755098</v>
+      </c>
+      <c r="L20">
+        <v>9.9923334088392401</v>
+      </c>
+      <c r="M20">
+        <v>19.784630249636098</v>
+      </c>
+      <c r="N20">
+        <v>15.309142963266799</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>73.599999999999994</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>11.1</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="2"/>
+        <v>18.5</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="K21">
+        <v>73.612159321677296</v>
+      </c>
+      <c r="L21">
+        <v>11.0836876677227</v>
+      </c>
+      <c r="M21">
+        <v>18.524551855844599</v>
+      </c>
+      <c r="N21">
+        <v>16.9811946942506</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="B22" s="6">
+        <f t="shared" si="0"/>
+        <v>77.900000000000006</v>
+      </c>
+      <c r="C22" s="6">
+        <f t="shared" si="1"/>
+        <v>12.2</v>
+      </c>
+      <c r="D22" s="6">
+        <f t="shared" si="2"/>
+        <v>17.2</v>
+      </c>
+      <c r="E22" s="6">
+        <f t="shared" si="3"/>
+        <v>18.7</v>
+      </c>
+      <c r="K22">
+        <v>77.942286340599495</v>
+      </c>
+      <c r="L22">
+        <v>12.1952083865195</v>
+      </c>
+      <c r="M22">
+        <v>17.2255412489904</v>
+      </c>
+      <c r="N22">
+        <v>18.6841432343425</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>82.3</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="1"/>
+        <v>13.3</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="2"/>
+        <v>15.9</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="3"/>
+        <v>20.399999999999999</v>
+      </c>
+      <c r="K23">
+        <v>82.272413359521707</v>
+      </c>
+      <c r="L23">
+        <v>13.319870070199901</v>
+      </c>
+      <c r="M23">
+        <v>15.893426556994401</v>
+      </c>
+      <c r="N23">
+        <v>20.407224900686799</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>86.6</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="1"/>
+        <v>14.5</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="2"/>
+        <v>14.5</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="3"/>
+        <v>22.1</v>
+      </c>
+      <c r="K24">
+        <v>86.602540378443905</v>
+      </c>
+      <c r="L24">
+        <v>14.450537235463001</v>
+      </c>
+      <c r="M24">
+        <v>14.5341595278545</v>
+      </c>
+      <c r="N24">
+        <v>22.139507498620699</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA4709E9-033C-402D-A318-CF53CCD511C2}">
+  <dimension ref="A1:H32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T12" sqref="T12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="C4">
+        <v>0.19</v>
+      </c>
+      <c r="D4">
+        <v>131</v>
+      </c>
+      <c r="E4">
+        <v>11.57</v>
+      </c>
+      <c r="F4">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>0.1</v>
+      </c>
+      <c r="B5">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="C5">
+        <v>0.19</v>
+      </c>
+      <c r="D5">
+        <v>143</v>
+      </c>
+      <c r="E5">
+        <v>11.52</v>
+      </c>
+      <c r="F5">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>0.2</v>
+      </c>
+      <c r="B6">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="C6">
+        <v>0.18</v>
+      </c>
+      <c r="D6">
+        <v>184</v>
+      </c>
+      <c r="E6">
+        <v>11.34</v>
+      </c>
+      <c r="F6">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>0.3</v>
+      </c>
+      <c r="B7">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="C7">
+        <v>0.18</v>
+      </c>
+      <c r="D7">
+        <v>197</v>
+      </c>
+      <c r="E7">
+        <v>11.1</v>
+      </c>
+      <c r="F7">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>0.4</v>
+      </c>
+      <c r="B8">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="C8">
+        <v>0.16</v>
+      </c>
+      <c r="D8">
+        <v>168</v>
+      </c>
+      <c r="E8">
+        <v>10.78</v>
+      </c>
+      <c r="F8">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>0.5</v>
+      </c>
+      <c r="B9">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="C9">
+        <v>0.16</v>
+      </c>
+      <c r="D9">
+        <v>200</v>
+      </c>
+      <c r="E9">
+        <v>10.5</v>
+      </c>
+      <c r="F9">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>0.6</v>
+      </c>
+      <c r="B10">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="C10">
+        <v>0.15</v>
+      </c>
+      <c r="D10">
+        <v>181</v>
+      </c>
+      <c r="E10">
+        <v>10.27</v>
+      </c>
+      <c r="F10">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>0.7</v>
+      </c>
+      <c r="B11">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="C11">
+        <v>0.15</v>
+      </c>
+      <c r="D11">
+        <v>210</v>
+      </c>
+      <c r="E11">
+        <v>10.23</v>
+      </c>
+      <c r="F11">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>0.8</v>
+      </c>
+      <c r="B12">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="C12">
+        <v>0.16</v>
+      </c>
+      <c r="D12">
+        <v>207</v>
+      </c>
+      <c r="E12">
+        <v>10.44</v>
+      </c>
+      <c r="F12">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>0.9</v>
+      </c>
+      <c r="B13">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="C13">
+        <v>0.17</v>
+      </c>
+      <c r="D13">
+        <v>206</v>
+      </c>
+      <c r="E13">
+        <v>10.9</v>
+      </c>
+      <c r="F13">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="C14">
+        <v>0.19</v>
+      </c>
+      <c r="D14">
+        <v>210</v>
+      </c>
+      <c r="E14">
+        <v>11.68</v>
+      </c>
+      <c r="F14">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="G21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>11.57</v>
+      </c>
+      <c r="C22">
+        <v>0.43547357157823002</v>
+      </c>
+      <c r="D22">
+        <f>B22/C22</f>
+        <v>26.568776511668343</v>
+      </c>
+      <c r="G22">
+        <v>12.303811788053601</v>
+      </c>
+      <c r="H22">
+        <f>ROUND(G22,1)</f>
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>11.52</v>
+      </c>
+      <c r="C23">
+        <v>0.43281602943595299</v>
+      </c>
+      <c r="D23">
+        <f t="shared" ref="D23:D32" si="0">B23/C23</f>
+        <v>26.616389450762473</v>
+      </c>
+      <c r="G23">
+        <v>12.228725949390901</v>
+      </c>
+      <c r="H23">
+        <f t="shared" ref="H23:H32" si="1">ROUND(G23,1)</f>
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>11.34</v>
+      </c>
+      <c r="C24">
+        <v>0.425189708052995</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>26.670448002910266</v>
+      </c>
+      <c r="G24">
+        <v>12.0132528895883</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>11.1</v>
+      </c>
+      <c r="C25">
+        <v>0.41364814597969302</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>26.834400463008301</v>
+      </c>
+      <c r="G25">
+        <v>11.6871591453103</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="1"/>
+        <v>11.7</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>10.78</v>
+      </c>
+      <c r="C26">
+        <v>0.399983676716897</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>26.951099826080995</v>
+      </c>
+      <c r="G26">
+        <v>11.3010850665005</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="1"/>
+        <v>11.3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>10.5</v>
+      </c>
+      <c r="C27">
+        <v>0.386728686302309</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>27.15081754186723</v>
+      </c>
+      <c r="G27">
+        <v>10.9265803480569</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="1"/>
+        <v>10.9</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>10.27</v>
+      </c>
+      <c r="C28">
+        <v>0.37702176128386899</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>27.23980696771363</v>
+      </c>
+      <c r="G28">
+        <v>10.652322192654299</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="1"/>
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>10.23</v>
+      </c>
+      <c r="C29">
+        <v>0.374186368003253</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>27.339317716435531</v>
+      </c>
+      <c r="G29">
+        <v>10.572211371822201</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="1"/>
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>10.44</v>
+      </c>
+      <c r="C30">
+        <v>0.38095883749769099</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>27.404535536108352</v>
+      </c>
+      <c r="G30">
+        <v>10.7635598150765</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="1"/>
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>10.9</v>
+      </c>
+      <c r="C31">
+        <v>0.39863255946114901</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>27.343476445411433</v>
+      </c>
+      <c r="G31">
+        <v>11.2629107810713</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="1"/>
+        <v>11.3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>11.68</v>
+      </c>
+      <c r="C32">
+        <v>0.42666558611074101</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>27.375069328812604</v>
+      </c>
+      <c r="G32">
+        <v>12.0549521499563</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="1"/>
+        <v>12.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>